<commit_message>
Major Change: Adapting solution on new approach
</commit_message>
<xml_diff>
--- a/LabelHelper.xlsx
+++ b/LabelHelper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Colab Notebooks\IndoorTrackingML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A2EDA6-FEB5-4835-8EA2-B2C6426C1B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA095F-4A89-4A55-80C2-C167ED515533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{E70BF270-188A-45FA-9620-AB456C9479E9}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Room2</t>
   </si>
   <si>
-    <t>OOB</t>
-  </si>
-  <si>
     <t>lasttimestamp</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>endzeit</t>
+  </si>
+  <si>
+    <t>Corridor</t>
   </si>
 </sst>
 </file>
@@ -140,13 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,14 +460,13 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -482,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -501,7 +496,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1679222510</v>
       </c>
       <c r="D2">
@@ -521,7 +516,7 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>1679222700</v>
       </c>
       <c r="D3">
@@ -541,7 +536,7 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1679222885</v>
       </c>
       <c r="D4">
@@ -561,7 +556,7 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>1679223080</v>
       </c>
       <c r="D5">
@@ -581,7 +576,7 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>1679224790</v>
       </c>
       <c r="D6">
@@ -599,12 +594,12 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7">
         <v>1679224000</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>1679224180</v>
       </c>
       <c r="E7" s="1">
@@ -619,9 +614,9 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+      <c r="C8">
         <v>1679224190</v>
       </c>
       <c r="D8">
@@ -641,7 +636,7 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>1679224380</v>
       </c>
       <c r="D9">
@@ -661,7 +656,7 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>1679221180</v>
       </c>
       <c r="D10">
@@ -674,43 +669,43 @@
         <v>0.47407407407407409</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
         <v>1679225750</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>1679225930</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>0.52488425925925919</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>0.52696759259259263</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>1679225940</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>1679226120</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>0.52708333333333335</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>0.52916666666666667</v>
       </c>
     </row>
@@ -721,7 +716,7 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>1679221690</v>
       </c>
       <c r="D13">

</xml_diff>